<commit_message>
Fixed error with calculating marginal taxes
</commit_message>
<xml_diff>
--- a/italy/italy-tax.xlsx
+++ b/italy/italy-tax.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicarapson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicarapson/Documents/GitHub/simulating-ubi-impacts/italy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD2B0B7-517F-F74B-85BB-8BFF40362193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312CDA21-2CBB-2646-ABDD-16BF00CA5374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="500" windowWidth="24000" windowHeight="17500" activeTab="2" xr2:uid="{288C6545-28DD-A54E-BD94-0F037A4122A4}"/>
+    <workbookView xWindow="4640" yWindow="500" windowWidth="24000" windowHeight="17500" xr2:uid="{288C6545-28DD-A54E-BD94-0F037A4122A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="2" r:id="rId1"/>
     <sheet name="Groups" sheetId="3" r:id="rId2"/>
     <sheet name="Example" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Gross Income</t>
   </si>
@@ -73,18 +73,12 @@
     <t>Calculation</t>
   </si>
   <si>
-    <t>Rate is 23% for €1,000 -15,000, 27% for €15,000-28,000, 38% for €28,000-55,000, 41% for €55,000-75,000, and 43% for over €75,000</t>
-  </si>
-  <si>
     <t>Imposta sul valore aggiunto</t>
   </si>
   <si>
     <t>IVA</t>
   </si>
   <si>
-    <t>Valued added tax</t>
-  </si>
-  <si>
     <t>https://taxsummaries.pwc.com/italy/individual/other-taxes</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
     <t>Staff, executive, self-employed, unemployed</t>
   </si>
   <si>
-    <t>For employes: total rate approximately 40% depending on position, 30% is charged to exployer and 10% to employee</t>
-  </si>
-  <si>
     <t>Social security contributions contributed by all workers; covers social security, unemployment, sickness, maternity, social mobility, and other funds</t>
   </si>
   <si>
@@ -184,15 +175,9 @@
     <t>PREVINDAI</t>
   </si>
   <si>
-    <t>Otto Per Mille</t>
-  </si>
-  <si>
     <t>OPM</t>
   </si>
   <si>
-    <t>Eight Per Thousand</t>
-  </si>
-  <si>
     <t>Assegno unico e universale per i figli a carico</t>
   </si>
   <si>
@@ -208,9 +193,6 @@
     <t>Marital Status</t>
   </si>
   <si>
-    <t>Single, unmarried partner, married</t>
-  </si>
-  <si>
     <t>https://www.inps.it/it/it/inps-comunica/atti/circolari-messaggi-e-normativa/dettaglio.circolari-e-messaggi.2023.04.circolare-numero-41-del-07-04-2023_14128.html</t>
   </si>
   <si>
@@ -218,6 +200,45 @@
   </si>
   <si>
     <t>0, 1, 2, 3, 4+</t>
+  </si>
+  <si>
+    <t>Complementary pension tax fund paid by executives</t>
+  </si>
+  <si>
+    <t>For employes: total rate approximately 40% depending on position, 30% is charged to employer and 10% to employee; for executives: 9.19% of annual income up to an income ceiling of €46,630, after marginal earnings are taxed at 10.19%</t>
+  </si>
+  <si>
+    <t>For executives: 1% of annual income up to an income of €59,224.54 and a maximum of €129.12 in yearly training charges</t>
+  </si>
+  <si>
+    <t>Assegno di Inclusione</t>
+  </si>
+  <si>
+    <t>ADI</t>
+  </si>
+  <si>
+    <t>Inclusion Cheques</t>
+  </si>
+  <si>
+    <t>Supporto alla Formazione e al Lavoro</t>
+  </si>
+  <si>
+    <t>SFL</t>
+  </si>
+  <si>
+    <t>Valued-added tax</t>
+  </si>
+  <si>
+    <t>Aid to Vocational Training</t>
+  </si>
+  <si>
+    <t>https://fiscomania.com/familiari-a-carico-limiti-detrazione/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marginal rate is 23% for €1,000 -15,000, 27% for €15,000-28,000, 38% for €28,000-55,000, 41% for €55,000-75,000, and 43% for over €75,000; exempt at less than €8,000 for employees and less than €4,800 for everyone, including unemployed; if spouse makes less than €2,840.51 </t>
+  </si>
+  <si>
+    <t>Single, unmarried partner, married one earner, marrier two earners</t>
   </si>
 </sst>
 </file>
@@ -615,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360BB8DA-47A3-0740-96F0-CBBF7BC23F54}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,7 +648,7 @@
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="124.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="198.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="203.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" hidden="1"/>
@@ -650,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -670,142 +691,189 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -814,8 +882,14 @@
     <hyperlink ref="F3" r:id="rId2" xr:uid="{C9EF3F1D-6AC4-DD4C-A498-DEE4B74AB72E}"/>
     <hyperlink ref="G3" r:id="rId3" xr:uid="{2DDE503A-98BC-EA46-8706-625EE624F5D4}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{50089640-C9A1-0D45-A8FF-A8B89EF316AD}"/>
-    <hyperlink ref="G11" r:id="rId5" xr:uid="{01A7AEF6-2B0B-6745-9334-C82123981607}"/>
-    <hyperlink ref="F11" r:id="rId6" location=":~:text=L'assegno%20va%20da%20un,massimo%20di%20%E2%82%AC%2085%2Fmese." xr:uid="{6C5CC200-E194-844D-943A-AF7AEB100928}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{01A7AEF6-2B0B-6745-9334-C82123981607}"/>
+    <hyperlink ref="F10" r:id="rId6" location=":~:text=L'assegno%20va%20da%20un,massimo%20di%20%E2%82%AC%2085%2Fmese." xr:uid="{6C5CC200-E194-844D-943A-AF7AEB100928}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{5118D276-FC89-D243-8642-D7501D5185E9}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{FB1696E1-28EC-3747-AEF2-2E65014CB6ED}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{A2FEAC64-22D6-744A-B235-52D72FB7DB2D}"/>
+    <hyperlink ref="F8" r:id="rId10" xr:uid="{03AB33A5-2C0F-8F4B-860C-EADA86801B75}"/>
+    <hyperlink ref="F9" r:id="rId11" xr:uid="{A004206E-0791-4143-B353-44AB3145432D}"/>
+    <hyperlink ref="G2" r:id="rId12" xr:uid="{46D0DD49-8D23-9042-968C-659BEEE42E47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -826,46 +900,46 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -877,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3782E3B-A00B-6747-93AC-3B3EDD1FC5F4}">
   <dimension ref="A1:O401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -888,6 +962,7 @@
     <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
@@ -899,40 +974,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Completed Italy simulation code
</commit_message>
<xml_diff>
--- a/italy/italy-tax.xlsx
+++ b/italy/italy-tax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicarapson/Documents/GitHub/simulating-ubi-impacts/italy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312CDA21-2CBB-2646-ABDD-16BF00CA5374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7DF418-FC77-9A42-8E7F-E11A83538423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="500" windowWidth="24000" windowHeight="17500" xr2:uid="{288C6545-28DD-A54E-BD94-0F037A4122A4}"/>
+    <workbookView xWindow="3860" yWindow="500" windowWidth="25620" windowHeight="17500" xr2:uid="{288C6545-28DD-A54E-BD94-0F037A4122A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>Gross Income</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Supporting Source</t>
   </si>
   <si>
-    <t>Staff, executive, self-employed, unemployed</t>
-  </si>
-  <si>
     <t>Social security contributions contributed by all workers; covers social security, unemployment, sickness, maternity, social mobility, and other funds</t>
   </si>
   <si>
@@ -202,15 +199,6 @@
     <t>0, 1, 2, 3, 4+</t>
   </si>
   <si>
-    <t>Complementary pension tax fund paid by executives</t>
-  </si>
-  <si>
-    <t>For employes: total rate approximately 40% depending on position, 30% is charged to employer and 10% to employee; for executives: 9.19% of annual income up to an income ceiling of €46,630, after marginal earnings are taxed at 10.19%</t>
-  </si>
-  <si>
-    <t>For executives: 1% of annual income up to an income of €59,224.54 and a maximum of €129.12 in yearly training charges</t>
-  </si>
-  <si>
     <t>Assegno di Inclusione</t>
   </si>
   <si>
@@ -235,17 +223,101 @@
     <t>https://fiscomania.com/familiari-a-carico-limiti-detrazione/</t>
   </si>
   <si>
-    <t xml:space="preserve">Marginal rate is 23% for €1,000 -15,000, 27% for €15,000-28,000, 38% for €28,000-55,000, 41% for €55,000-75,000, and 43% for over €75,000; exempt at less than €8,000 for employees and less than €4,800 for everyone, including unemployed; if spouse makes less than €2,840.51 </t>
-  </si>
-  <si>
     <t>Single, unmarried partner, married one earner, marrier two earners</t>
+  </si>
+  <si>
+    <t>A national medical fund paid by executives</t>
+  </si>
+  <si>
+    <t>For executives: 1.87% of annual income with a yearly maximum €45,940</t>
+  </si>
+  <si>
+    <t>For executives: requirement to contribute at least €464.81</t>
+  </si>
+  <si>
+    <t>Complementary pension fund paid by executives; associated with companies and organisations</t>
+  </si>
+  <si>
+    <t>Complementary pension fund paid by executives; associated with insurance companies and financial institutions</t>
+  </si>
+  <si>
+    <t>A medical care fund paid by executives</t>
+  </si>
+  <si>
+    <t>An additional pension fund paid by executives</t>
+  </si>
+  <si>
+    <t>An economic contribution aimed at families with dependent children</t>
+  </si>
+  <si>
+    <t>Economic support and social and professional inclusion , conditional on means testing; paid through rechargeable electronic payments for maximum 18 months</t>
+  </si>
+  <si>
+    <t>For familes with at least one disabled, underage, elderly over 60 years of age, or disadvantaged condition (e.g. psychiatric patient): €6,000 or €7,560 per year if the family unit is made up of people all aged 67 or over or of people aged over 67 years of age and by other family members all in conditions of serious disability or non-self-sufficiency; can cover rent €3,360 €1,800 euros per year  if the family unit is made up of people all aged 67 or over or of people aged 67 or over and other family non-self-sufficient; employment over €3,000 per year makes benefit cumulative</t>
+  </si>
+  <si>
+    <t>https://www.fiscoetasse.com/rassegna-stampa/33738-assegno-inclusione-2024-tutte-le-regole-e-calendario-pagamenti.html#:~:text=Assegno%20di%20inclusione%3A%20importo%2C%20durata&amp;text=L'assegno%20di%20inclusione%20dura,che%20andranno%20comunicati%20all'INPS.</t>
+  </si>
+  <si>
+    <t>https://www.lavoro.gov.it/temi-e-priorita/decreto-lavoro/Pagine/assegno-di-inclusione#:~:text=L'importo%20dell'Assegno%20di,familiari%20tutti%20in%20condizioni%20di</t>
+  </si>
+  <si>
+    <t>Support for training and work for a maximum of 12 months</t>
+  </si>
+  <si>
+    <t>For those seeking work: €350 euros per month provided annual income is under €6,000</t>
+  </si>
+  <si>
+    <t>https://www.ticonsiglio.com/supporto-formazione-lavoro/#:~:text=Il%20Supporto%20per%20la%20formazione%20e%20il%20lavoro%20ha%20un,anno%2C%20e%20non%20%C3%A8%20rinnovabile.</t>
+  </si>
+  <si>
+    <t>Employee, executive, self-employed, unemployed</t>
+  </si>
+  <si>
+    <r>
+      <t>Marginal rate is 23% for €1,000 -15,000, 27% for €15,000-28,000, 38% for €28,000-55,000, 41% for €55,000-75,000, and 43% for over €75,000; exempt at less than €8,000 for employees and less than €4,800 for everyone, including unemployed; if spouse makes less than €2,840.51 deduction €800 if household income is less than €15,000; €690 if greater than €15,000 but less than €40,000, and equal to 800 – [110 × (total income/15,000)] for income under €15,000 with an added€10 for €29,000-29,199, €20 for €29,200-34,699; €30 for €34,700-34,999; €20 for €35,000-35,099; €10 for €35,100-35,199; between €40,000 and €80,000 equal to 690 × [(80,000 – total income)/40,000];</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> if dependent children over 24 make less than €2,840.51 (or €4,000 for children under 24); can deduct €950 for each non-disabled child, €1,350 for each disabled child;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (no deductions for children under 21, as these are covered by AUUFC); for married parents deductions are split 50% or 100% to the parent with the highest income</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.globalvatcompliance.com/vat-rates-in-italy/</t>
+  </si>
+  <si>
+    <t>For executives: set at a tax level of 4 percent of income only for those with maximum annual income €180,000</t>
+  </si>
+  <si>
+    <t>For executives: set at a flat rate of €1,120</t>
+  </si>
+  <si>
+    <t>For executives: 1% of annual income up to an income of €59,224.54 and a maximum of €130.00 in yearly training charges</t>
+  </si>
+  <si>
+    <t>For employees: total rate approximately 40% depending on position, 30% is charged to employer and 10% to employee; for executives: 9.19% of annual income up to an income ceiling of €55,008, after marginal earnings are taxed at 10.19%</t>
+  </si>
+  <si>
+    <t>A minimum of €50/month to a maximum of €175/month for each dependent child under 18; for dependent children aged between 18 and 21 a minimum of €25/month to a maximum of €85/month; amounts increase by 50% for children under one year, increase by 50%  if three or more children provided that they have household income under  €40,000; increase by 50% if at least four children; increase of  €20 per child-month for mothers under 21; increase of  €30 per child-month for children under 18 if both parents have work income provided household income is under  €15,000 (bonus progressively reduces until household income of  €40,000)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +336,16 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,11 +378,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,242 +737,296 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360BB8DA-47A3-0740-96F0-CBBF7BC23F54}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="124.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="203.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" hidden="1"/>
+    <col min="1" max="1" width="38.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="E5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="D11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -883,13 +1036,16 @@
     <hyperlink ref="G3" r:id="rId3" xr:uid="{2DDE503A-98BC-EA46-8706-625EE624F5D4}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{50089640-C9A1-0D45-A8FF-A8B89EF316AD}"/>
     <hyperlink ref="G10" r:id="rId5" xr:uid="{01A7AEF6-2B0B-6745-9334-C82123981607}"/>
-    <hyperlink ref="F10" r:id="rId6" location=":~:text=L'assegno%20va%20da%20un,massimo%20di%20%E2%82%AC%2085%2Fmese." xr:uid="{6C5CC200-E194-844D-943A-AF7AEB100928}"/>
-    <hyperlink ref="F5" r:id="rId7" xr:uid="{5118D276-FC89-D243-8642-D7501D5185E9}"/>
-    <hyperlink ref="F6" r:id="rId8" xr:uid="{FB1696E1-28EC-3747-AEF2-2E65014CB6ED}"/>
-    <hyperlink ref="F7" r:id="rId9" xr:uid="{A2FEAC64-22D6-744A-B235-52D72FB7DB2D}"/>
-    <hyperlink ref="F8" r:id="rId10" xr:uid="{03AB33A5-2C0F-8F4B-860C-EADA86801B75}"/>
-    <hyperlink ref="F9" r:id="rId11" xr:uid="{A004206E-0791-4143-B353-44AB3145432D}"/>
-    <hyperlink ref="G2" r:id="rId12" xr:uid="{46D0DD49-8D23-9042-968C-659BEEE42E47}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{5118D276-FC89-D243-8642-D7501D5185E9}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{FB1696E1-28EC-3747-AEF2-2E65014CB6ED}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{A2FEAC64-22D6-744A-B235-52D72FB7DB2D}"/>
+    <hyperlink ref="F8" r:id="rId9" xr:uid="{03AB33A5-2C0F-8F4B-860C-EADA86801B75}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{A004206E-0791-4143-B353-44AB3145432D}"/>
+    <hyperlink ref="G2" r:id="rId11" xr:uid="{46D0DD49-8D23-9042-968C-659BEEE42E47}"/>
+    <hyperlink ref="F10" r:id="rId12" location=":~:text=L'assegno%20va%20da%20un,massimo%20di%20%E2%82%AC%2085%2Fmese." xr:uid="{1BCD480C-2E2E-184E-8436-EECFC8D2E108}"/>
+    <hyperlink ref="G11" r:id="rId13" location=":~:text=Assegno%20di%20inclusione%3A%20importo%2C%20durata&amp;text=L'assegno%20di%20inclusione%20dura,che%20andranno%20comunicati%20all'INPS." display="https://www.fiscoetasse.com/rassegna-stampa/33738-assegno-inclusione-2024-tutte-le-regole-e-calendario-pagamenti.html#:~:text=Assegno%20di%20inclusione%3A%20importo%2C%20durata&amp;text=L'assegno%20di%20inclusione%20dura,che%20andranno%20comunicati%20all'INPS." xr:uid="{CB54428F-BC8D-1A41-80F4-75FBE17D342A}"/>
+    <hyperlink ref="F11" r:id="rId14" location=":~:text=L'importo%20dell'Assegno%20di,familiari%20tutti%20in%20condizioni%20di" xr:uid="{0C9A6CB6-5C96-3044-B773-97326AAC7E30}"/>
+    <hyperlink ref="F12" r:id="rId15" location=":~:text=Il%20Supporto%20per%20la%20formazione%20e%20il%20lavoro%20ha%20un,anno%2C%20e%20non%20%C3%A8%20rinnovabile." xr:uid="{698A2C1B-4B85-8348-A0B6-78D819F53153}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -900,7 +1056,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -923,23 +1079,23 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -980,25 +1136,25 @@
         <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>22</v>

</xml_diff>